<commit_message>
Varmaan kamalaa koodia mutta nyt on excelissä rivi, joka näyttää hyvältä
</commit_message>
<xml_diff>
--- a/strava_activity.xlsx
+++ b/strava_activity.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,35 +442,40 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Distance (m)</t>
+          <t>Distance (km)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Moving Time (s)</t>
+          <t>Moving Time (h:min)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Moving Time (seconds)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Elapsed Time (s)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Start Date</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Average Speed (m/s)</t>
-        </is>
-      </c>
       <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Average Speed (min/km)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Max Speed (m/s)</t>
         </is>
@@ -483,29 +488,36 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4577.9</v>
-      </c>
-      <c r="C2" t="n">
-        <v>4331</v>
+        <v>4.58</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>01:12:11</t>
+        </is>
       </c>
       <c r="D2" t="n">
         <v>4331</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" t="n">
+        <v>4331</v>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>Run</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>2025-06-09T19:33:18Z</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>1.057</v>
-      </c>
-      <c r="H2" t="n">
-        <v>7.28</v>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>11.71602432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nyt saadaan vietyä data exceliin halutussa muodossa, tietyllä aikavälillä
</commit_message>
<xml_diff>
--- a/strava_activity.xlsx
+++ b/strava_activity.xlsx
@@ -7,8 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Activity" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Athlete Info" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Activities" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,22 +483,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Säbä</t>
+          <t>Lunch Run</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.58</v>
+        <v>1.87</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01:12:11</t>
+          <t>00:09:38</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4331</v>
+        <v>578</v>
       </c>
       <c r="E2" t="n">
-        <v>4331</v>
+        <v>617</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -508,77 +507,172 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-06-09T19:33:18Z</t>
+          <t>2025-05-29T11:14:02Z</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>05:09</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>11.71602432</v>
+        <v>6.759244800000001</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Athlete Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Athlete ID</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>City</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Country</t>
-        </is>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Intervalli</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8.41</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>00:39:55</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>2395</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2406</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-05-28T17:21:32Z</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>04:45</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>9.269821439999999</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Juho Tepponen</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>125339379</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Jyväskylä</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Finland</t>
-        </is>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Afternoon Run</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1.86</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>00:09:45</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>585</v>
+      </c>
+      <c r="E4" t="n">
+        <v>588</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-05-28T17:09:18Z</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>05:15</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>6.85580544</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Afternoon Run</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>12.05</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>01:09:35</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4175</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4440</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025-05-26T14:12:50Z</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>05:46</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>10.729496448</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Aloitus</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>10.63</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>01:00:53</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>3653</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3677</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025-05-21T12:08:53Z</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>05:44</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>6.40518912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nyt excel alkaa jo näyttämään hyvältä. Lisätty myös sykkeet, vanhoihin aktiviteetteihin ei saa sykkeitä, koska stravalla ei ole ollut oikeuksia
</commit_message>
<xml_diff>
--- a/strava_activity.xlsx
+++ b/strava_activity.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,26 +479,31 @@
           <t>Max Speed (m/s)</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Average Heart rate (b/min)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Lunch Run</t>
+          <t>Evening Run</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.87</v>
+        <v>15.5</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>00:09:38</t>
+          <t>01:34:05</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>578</v>
+        <v>5645</v>
       </c>
       <c r="E2" t="n">
-        <v>617</v>
+        <v>5850</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -507,37 +512,40 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-05-29T11:14:02Z</t>
+          <t>2025-06-29T18:01:37Z</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>05:09</t>
+          <t>06:04</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>6.759244800000001</v>
+        <v>14.348911104</v>
+      </c>
+      <c r="J2" t="n">
+        <v>149.3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Intervalli</t>
+          <t>Intervallit</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8.41</v>
+        <v>10.27</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>00:39:55</t>
+          <t>00:46:54</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2395</v>
+        <v>2814</v>
       </c>
       <c r="E3" t="n">
-        <v>2406</v>
+        <v>2867</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -546,37 +554,40 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-05-28T17:21:32Z</t>
+          <t>2025-06-26T17:15:08Z</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>04:45</t>
+          <t>04:34</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>9.269821439999999</v>
+        <v>10.87916544</v>
+      </c>
+      <c r="J3" t="n">
+        <v>168.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Afternoon Run</t>
+          <t>Säbä</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.86</v>
+        <v>7.42</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>00:09:45</t>
+          <t>01:35:30</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>585</v>
+        <v>5730</v>
       </c>
       <c r="E4" t="n">
-        <v>588</v>
+        <v>6304</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -585,16 +596,19 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-05-28T17:09:18Z</t>
+          <t>2025-06-23T19:03:11Z</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>05:15</t>
+          <t>12:52</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>6.85580544</v>
+        <v>11.39415552</v>
+      </c>
+      <c r="J4" t="n">
+        <v>144.2</v>
       </c>
     </row>
     <row r="5">
@@ -604,18 +618,18 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.05</v>
+        <v>7.84</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01:09:35</t>
+          <t>00:36:20</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4175</v>
+        <v>2180</v>
       </c>
       <c r="E5" t="n">
-        <v>4440</v>
+        <v>2187</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -624,37 +638,40 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-05-26T14:12:50Z</t>
+          <t>2025-06-22T15:48:10Z</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>05:46</t>
+          <t>04:38</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>10.729496448</v>
+        <v>7.7248512</v>
+      </c>
+      <c r="J5" t="n">
+        <v>166.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Aloitus</t>
+          <t>Afternoon Run</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>10.63</v>
+        <v>13.63</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01:00:53</t>
+          <t>01:21:54</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3653</v>
+        <v>4914</v>
       </c>
       <c r="E6" t="n">
-        <v>3677</v>
+        <v>4934</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -663,17 +680,262 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-05-21T12:08:53Z</t>
+          <t>2025-06-18T16:37:50Z</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>05:44</t>
+          <t>06:01</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>6.40518912</v>
-      </c>
+        <v>6.9201792</v>
+      </c>
+      <c r="J6" t="n">
+        <v>152.5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Evening Run</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>01:16:24</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>4584</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4584</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2025-06-16T19:27:54Z</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>16:15</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>8.78701824</v>
+      </c>
+      <c r="J7" t="n">
+        <v>142.4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Afternoon Run</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>00:20:36</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1236</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1242</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2025-06-15T13:01:30Z</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>05:57</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>6.66268416</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Säbä</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4.58</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>01:12:11</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>4331</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4331</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2025-06-09T19:33:18Z</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>15:46</t>
+        </is>
+      </c>
+      <c r="I9" t="n">
+        <v>11.71602432</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Afternoon Run</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>7.19</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>00:47:31</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>2851</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2909</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2025-06-04T16:29:24Z</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>06:37</t>
+        </is>
+      </c>
+      <c r="I10" t="n">
+        <v>6.46956288</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Intervalli</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>9.539999999999999</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>00:44:31</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>2671</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2806</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2025-06-03T17:53:51Z</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>04:40</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>10.39636224</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Lunch Run</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>16.28</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>01:44:35</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>6275</v>
+      </c>
+      <c r="E12" t="n">
+        <v>6876</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Run</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2025-06-01T12:37:04Z</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>06:25</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>7.892222976</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>